<commit_message>
add 001632 model parameter
</commit_message>
<xml_diff>
--- a/parameter.xlsx
+++ b/parameter.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn\Allen\code\gitee_project\find_found\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810CB291-853A-444F-B381-2A78EB074C17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE18B24-5F50-4260-804C-FE60619A90BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="3555" windowWidth="16230" windowHeight="11595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19035" yWindow="2190" windowWidth="16230" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,11 +72,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>linear</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mape</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F4"/>
+  <dimension ref="B3:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -447,6 +447,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1632</v>
+      </c>
+      <c r="C5">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -456,15 +473,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93AF87B4-D4FC-4E72-A1BE-9E70ECF87BF7}">
-  <dimension ref="B2:F5"/>
+  <dimension ref="B2:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -481,12 +498,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1632</v>
       </c>
       <c r="C3">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -498,36 +515,61 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C4">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C5">
+        <v>256</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <f>J5+K6</f>
+        <v>320</v>
+      </c>
+      <c r="K6">
         <v>64</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <f>J6+K6</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <f>J7+K6</f>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>